<commit_message>
Cập nhật API Login
</commit_message>
<xml_diff>
--- a/03.Design/API.xlsx
+++ b/03.Design/API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>List API:</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve"> "error_code" : "1",</t>
   </si>
   <si>
-    <t xml:space="preserve"> "message" : "login fail"</t>
-  </si>
-  <si>
     <t>Đăng nhập thành công</t>
   </si>
   <si>
@@ -201,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "wrong password"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "wrong email"</t>
   </si>
 </sst>
 </file>
@@ -281,8 +284,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -583,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -593,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -626,13 +657,13 @@
     </row>
     <row r="6" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -643,10 +674,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -676,12 +707,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -692,7 +723,7 @@
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -707,12 +738,12 @@
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -722,7 +753,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -737,7 +768,7 @@
     </row>
     <row r="18" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -749,13 +780,24 @@
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -778,7 +820,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -788,7 +830,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -798,42 +840,42 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -844,7 +886,7 @@
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -859,12 +901,12 @@
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -874,7 +916,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -889,7 +931,7 @@
     </row>
     <row r="25" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -918,7 +960,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -928,7 +970,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -938,42 +980,42 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -984,7 +1026,7 @@
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -999,12 +1041,12 @@
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1014,7 +1056,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1029,7 +1071,7 @@
     </row>
     <row r="25" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1058,7 +1100,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1068,7 +1110,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1078,7 +1120,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1094,42 +1136,42 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1164,7 +1206,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1174,7 +1216,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1184,7 +1226,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1195,7 +1237,7 @@
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1210,17 +1252,17 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1230,7 +1272,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1245,7 +1287,7 @@
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
code màn hình login & register + update api + code web php login & register
</commit_message>
<xml_diff>
--- a/03.Design/API.xlsx
+++ b/03.Design/API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Edit" sheetId="4" r:id="rId4"/>
     <sheet name="Information" sheetId="7" r:id="rId5"/>
     <sheet name="Reminder" sheetId="8" r:id="rId6"/>
+    <sheet name="More" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
   <si>
     <t>List API:</t>
   </si>
@@ -107,9 +108,6 @@
     <t>- năm sinh : int</t>
   </si>
   <si>
-    <t xml:space="preserve"> "message" : "register fail"</t>
-  </si>
-  <si>
     <t>Đăng ký thành công</t>
   </si>
   <si>
@@ -164,12 +162,6 @@
     <t xml:space="preserve"> "email" : "####",</t>
   </si>
   <si>
-    <t xml:space="preserve"> "message" : "register success",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "message" : "login success",</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "message" : "edit success",</t>
   </si>
   <si>
@@ -200,10 +192,43 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve"> "message" : "wrong password"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "message" : "wrong email"</t>
+    <t xml:space="preserve"> "token" : "####"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "User Successfully logged",</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "Wrong email"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "Wrong password"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "Email exist"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "message" : "Sign Up Successful",</t>
+  </si>
+  <si>
+    <t>MORE</t>
+  </si>
+  <si>
+    <t>Khi gửi password lên server, password sẽ được mã hóa trên server và lưu vào database.</t>
+  </si>
+  <si>
+    <t>Khi Client đăng nhập thành công sẽ lưu lại 1 biến Token, từ đó về sau mỗi lần khởi động App, Client sẽ gửi Token lên server để kiểm tra thay vì gửi Email và Password.</t>
+  </si>
+  <si>
+    <t>Tạo thêm 1 đường link cung cấp tổng số Image Target mà server đã có, do trên Vuforia Cloud không hỗ trợ hàm đếm cái này</t>
+  </si>
+  <si>
+    <t>{"1":"Tân Mai", "2":"Tân Định", "4":"Trương Định", "5":"Thăng Long", "7":"Bách Khoa"}</t>
+  </si>
+  <si>
+    <t>{ "total" : "123" }</t>
+  </si>
+  <si>
+    <t>Tạo thêm 1 đường link cung cấp danh sách trường học từ bảng School (public thông tin)</t>
   </si>
 </sst>
 </file>
@@ -614,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -657,13 +682,13 @@
     </row>
     <row r="6" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -676,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -738,12 +763,12 @@
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -768,7 +793,7 @@
     </row>
     <row r="18" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -810,7 +835,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -886,7 +911,7 @@
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -901,7 +926,7 @@
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -916,7 +941,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -931,7 +956,7 @@
     </row>
     <row r="25" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -949,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -960,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -970,7 +995,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1026,7 +1051,7 @@
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1041,7 +1066,7 @@
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1056,7 +1081,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1071,7 +1096,7 @@
     </row>
     <row r="25" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1090,7 +1115,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1125,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1110,7 +1135,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1136,42 +1161,42 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1196,7 +1221,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1231,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1216,7 +1241,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1237,7 +1262,7 @@
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1252,17 +1277,17 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1272,7 +1297,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1287,7 +1312,7 @@
     </row>
     <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1308,4 +1333,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="32.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>